<commit_message>
revisi excel + perpanjangan
</commit_message>
<xml_diff>
--- a/requirement/siswatest.xlsx
+++ b/requirement/siswatest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VFAIROH\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1752EA-A5C0-4538-83D6-CFAEC8ED9A62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3AD96C-C50C-46CE-BAD5-E04750987B8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{486C2FB2-28FE-4C13-B9B8-6A90390025AD}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>nis</t>
   </si>
@@ -64,6 +64,42 @@
   </si>
   <si>
     <t>farhan</t>
+  </si>
+  <si>
+    <t>Jurusan</t>
+  </si>
+  <si>
+    <t>Inisial Jurusan</t>
+  </si>
+  <si>
+    <t>Tahun</t>
+  </si>
+  <si>
+    <t>web programming</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>wp</t>
+  </si>
+  <si>
+    <t>wb 1</t>
+  </si>
+  <si>
+    <t>akuntansi</t>
+  </si>
+  <si>
+    <t>ak</t>
+  </si>
+  <si>
+    <t>wb 2</t>
+  </si>
+  <si>
+    <t>software engineer</t>
+  </si>
+  <si>
+    <t>se</t>
   </si>
 </sst>
 </file>
@@ -415,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4670E6C-AEA8-4229-8B70-C5AF43630872}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +462,7 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,10 +470,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4817040424</v>
       </c>
@@ -445,10 +493,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>2017</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1322347455</v>
       </c>
@@ -456,10 +516,22 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>2017</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8417040401</v>
       </c>
@@ -467,10 +539,22 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>2017</v>
+      </c>
+      <c r="F4" t="s">
         <v>6</v>
       </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1234567868</v>
       </c>
@@ -478,10 +562,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>2017</v>
+      </c>
+      <c r="F5" t="s">
         <v>8</v>
       </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8765532457</v>
       </c>
@@ -489,7 +585,19 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>2017</v>
+      </c>
+      <c r="F6" t="s">
         <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>